<commit_message>
update tuvung it 0801
</commit_message>
<xml_diff>
--- a/TuVung.xlsx
+++ b/TuVung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/dangtan_ngo2_dxc_com/Documents/Documents/Japanese/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DANG\studyingJapanese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1867" documentId="8_{B3EF4492-3947-4889-BFE5-1DC300788405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB401BB4-D55D-41C0-893A-BBEB57CED5AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9B2405-E9FD-4D4A-80B7-293F6A025480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B0E4D7E1-AC8C-4A97-A943-EDCC3B3B5427}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$497</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="1069">
   <si>
     <t>機能</t>
   </si>
@@ -3675,6 +3675,120 @@
     <t>わりあて「CÁT ĐƯƠNG」 phân chia, phân bổ, hoặc chỉ định
 各メンバーにタスクの割当を行った。
 Đã phân công nhiệm vụ cho từng thành viên.</t>
+  </si>
+  <si>
+    <t>余計</t>
+  </si>
+  <si>
+    <t>プランアーカイブ</t>
+  </si>
+  <si>
+    <t>Plan Archive - Lưu trữ kế hoạch</t>
+  </si>
+  <si>
+    <t>署名</t>
+  </si>
+  <si>
+    <t>自体</t>
+  </si>
+  <si>
+    <t>ブラウザ</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>ナビログデータ</t>
+  </si>
+  <si>
+    <t>Navigation log data - Dữ liệu nhật ký điều hướng</t>
+  </si>
+  <si>
+    <t>キャリア</t>
+  </si>
+  <si>
+    <t>career - Sự nghiệp</t>
+  </si>
+  <si>
+    <t>同期</t>
+  </si>
+  <si>
+    <t>乗継</t>
+  </si>
+  <si>
+    <t>繰り返し</t>
+  </si>
+  <si>
+    <t>切り捨て</t>
+  </si>
+  <si>
+    <t>切り上げ</t>
+  </si>
+  <si>
+    <t>無視</t>
+  </si>
+  <si>
+    <t>あらかじめ</t>
+  </si>
+  <si>
+    <t>生じる</t>
+  </si>
+  <si>
+    <t>よけい「DƯ KẾ」 dư thừa không cần thiết
+余計なことを言わないでください。
+→ Đừng nói những điều không cần thiết.</t>
+  </si>
+  <si>
+    <t>しょめい「THỰ DANH」 chữ ký
+契約書に署名をする必要があります。
+→ Cần phải ký vào hợp đồng.</t>
+  </si>
+  <si>
+    <t>じたい「TỰ THỂ」 chính bản thân (cái đó), tự nó, bản thân sự việc đó
+この計画自体に問題がある。
+→ Có vấn đề ngay trong chính kế hoạch này.</t>
+  </si>
+  <si>
+    <t>どうき「ĐỒNG KÌ」 cùng thời điểm, đồng bộ hóa
+彼は私の会社の同期です。
+→ Anh ấy là người vào công ty cùng đợt với tôi.
+スマホとパソコンを同期する。
+→ Đồng bộ điện thoại với máy tính.</t>
+  </si>
+  <si>
+    <t>のりつぎ「THỪA KẾ」 chuyển tiếp phương tiện, chuyển tàu
+乗継案内を確認してください。
+→ Vui lòng kiểm tra hướng dẫn chuyển tuyến.</t>
+  </si>
+  <si>
+    <t>くりかえし「SÀO PHẢN」 sự lặp lại, lặp đi lặp lại
+繰り返し練習することが大切です。
+→ Việc luyện tập lặp đi lặp lại là rất quan trọng.</t>
+  </si>
+  <si>
+    <t>きりすて「THIẾT XÁ」 làm tròn, bỏ phần dư
+3.9を切り捨てると3になる。
+→ Làm tròn 3.9 xuống thì thành 3.</t>
+  </si>
+  <si>
+    <t>きりあげ「THIẾT THƯỢNG」 làm tròn lên
+3.2を切り上げると4になる。
+→ Làm tròn 3.2 lên thì thành 4.</t>
+  </si>
+  <si>
+    <t>むし「VÔ THỊ」 phớt lờ, bỏ qua, hoặc làm ngơ
+ 彼は私の話を無視した。
+→ Anh ấy đã phớt lờ lời tôi nói.</t>
+  </si>
+  <si>
+    <t>予め あらかじめ 「DƯ」 trước, sẵn trước, hoặc làm gì đó từ trước để chuẩn bị.
+あらかじめ連絡しておいてください。
+→ Vui lòng liên lạc trước.</t>
+  </si>
+  <si>
+    <t>しょうじる「SANH」 (V2, tha V + ố) phát sinh, nảy sinh, hoặc xảy ra. Thường dùng trong ngữ cảnh trang trọng.
+問題が生じた場合は、すぐに報告してください。
+→ Nếu phát sinh vấn đề, hãy báo cáo ngay.</t>
   </si>
 </sst>
 </file>
@@ -3738,12 +3852,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -3764,7 +3884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3775,17 +3895,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4137,11 +4268,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572AC1B0-BE23-45AF-BF40-510643C6C658}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B558"/>
+  <dimension ref="A1:B593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A556" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A558" sqref="A558"/>
+      <pane ySplit="1" topLeftCell="A571" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F571" sqref="F571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7784,7 +7915,7 @@
       </c>
     </row>
     <row r="484" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A484" s="9" t="s">
+      <c r="A484" s="8" t="s">
         <v>891</v>
       </c>
       <c r="B484" s="1" t="s">
@@ -7960,7 +8091,7 @@
       </c>
     </row>
     <row r="506" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A506" s="10" t="s">
+      <c r="A506" s="9" t="s">
         <v>934</v>
       </c>
       <c r="B506" s="1" t="s">
@@ -8032,7 +8163,7 @@
       </c>
     </row>
     <row r="515" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A515" s="11" t="s">
+      <c r="A515" s="10" t="s">
         <v>950</v>
       </c>
       <c r="B515" s="1" t="s">
@@ -8040,7 +8171,7 @@
       </c>
     </row>
     <row r="516" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A516" s="11" t="s">
+      <c r="A516" s="10" t="s">
         <v>952</v>
       </c>
       <c r="B516" s="1" t="s">
@@ -8096,7 +8227,7 @@
       </c>
     </row>
     <row r="523" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A523" s="11" t="s">
+      <c r="A523" s="10" t="s">
         <v>968</v>
       </c>
       <c r="B523" s="1" t="s">
@@ -8264,7 +8395,7 @@
       </c>
     </row>
     <row r="544" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A544" s="8" t="s">
+      <c r="A544" s="11" t="s">
         <v>1010</v>
       </c>
       <c r="B544" s="1" t="s">
@@ -8383,11 +8514,137 @@
         <v>1038</v>
       </c>
     </row>
+    <row r="559" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A559" s="12" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" s="2" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A561" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A562" s="2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="563" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A563" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A564" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A565" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A566" s="2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="567" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A567" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A569" s="2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A570" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A571" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A572" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A573" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="593" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B593" s="1"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B497" xr:uid="{572AC1B0-BE23-45AF-BF40-510643C6C658}"/>
-  <conditionalFormatting sqref="A485:A505 A1:A483 A507:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  <conditionalFormatting sqref="A1:A558 A593:A1048576 A560:A573">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A485:A505 A1:A483 A507:A558 A593:A1048576 A560:A573">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A238" xr:uid="{103D1572-9A6E-4A56-99B1-E430078D44EF}">

</xml_diff>